<commit_message>
Fix correct parsing of typed excel cells
</commit_message>
<xml_diff>
--- a/test/files/WithHeaderAndTabs.xlsx
+++ b/test/files/WithHeaderAndTabs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michi/git/file-glance/test/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeldell/git/file-glance/test/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098D5F37-93AA-384D-BD19-52E29FF50B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DCA566-A871-CF4A-A297-9D276C89236D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="76800" windowHeight="42700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="136">
   <si>
     <t>ISIN</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Share Issuer</t>
   </si>
   <si>
-    <t>LEI of Share Issuer</t>
-  </si>
-  <si>
     <t>Net Short Position (%)</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>AMPLIFON SPA</t>
   </si>
   <si>
-    <t>ZYXJDNVM2JI3VBM8G556</t>
-  </si>
-  <si>
     <t>IT0004056880</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>BANCA MONTE DEI PASCHI DI SIENA SPA</t>
   </si>
   <si>
-    <t>J4CP7MHCXR8DAQMKIL78</t>
-  </si>
-  <si>
     <t>IT0005508921</t>
   </si>
   <si>
@@ -89,9 +80,6 @@
     <t>BIESSE SPA</t>
   </si>
   <si>
-    <t>815600C41423BF4CC386</t>
-  </si>
-  <si>
     <t>IT0003097257</t>
   </si>
   <si>
@@ -104,9 +92,6 @@
     <t>BIO-ON spa</t>
   </si>
   <si>
-    <t>8156001A4CBBB7B42E94</t>
-  </si>
-  <si>
     <t>IT0005056236</t>
   </si>
   <si>
@@ -125,9 +110,6 @@
     <t>CNH INDUSTRIAL NV</t>
   </si>
   <si>
-    <t>549300WGC2HZ5J67V817</t>
-  </si>
-  <si>
     <t>NL0010545661</t>
   </si>
   <si>
@@ -140,9 +122,6 @@
     <t>DIASORIN SPA</t>
   </si>
   <si>
-    <t>8156002878BDF0EE4348</t>
-  </si>
-  <si>
     <t>IT0003492391</t>
   </si>
   <si>
@@ -155,9 +134,6 @@
     <t>DIGITAL BROS SPA</t>
   </si>
   <si>
-    <t>815600D581F8552C4F54</t>
-  </si>
-  <si>
     <t>IT0001469995</t>
   </si>
   <si>
@@ -176,9 +152,6 @@
     <t>DoVALUE SPA</t>
   </si>
   <si>
-    <t>8156007AF7DB5FE05555</t>
-  </si>
-  <si>
     <t>IT0001044996</t>
   </si>
   <si>
@@ -200,18 +173,12 @@
     <t>ERG SPA</t>
   </si>
   <si>
-    <t>8156004604684CA44A90</t>
-  </si>
-  <si>
     <t>IT0001157020</t>
   </si>
   <si>
     <t>EUROGROUP LAMINATIONS SPA</t>
   </si>
   <si>
-    <t>8156004FC8565D73AE78</t>
-  </si>
-  <si>
     <t>IT0005527616</t>
   </si>
   <si>
@@ -230,9 +197,6 @@
     <t>EUROTECH SPA</t>
   </si>
   <si>
-    <t>815600B283DC6683D832</t>
-  </si>
-  <si>
     <t>IT0003895668</t>
   </si>
   <si>
@@ -245,45 +209,30 @@
     <t>FINCANTIERI SPA</t>
   </si>
   <si>
-    <t>8156005BDF49128B6239</t>
-  </si>
-  <si>
     <t>IT0001415246</t>
   </si>
   <si>
     <t>FINECOBANK BANCA FINECO S.P.A.</t>
   </si>
   <si>
-    <t>549300L7YCATGO57ZE10</t>
-  </si>
-  <si>
     <t>IT0000072170</t>
   </si>
   <si>
     <t>IGD - IMMOBILIARE GRANDE DISTRIBUZIONE SIIQ SPA</t>
   </si>
   <si>
-    <t>815600CF8C0389D0E272</t>
-  </si>
-  <si>
     <t>IT0005322612</t>
   </si>
   <si>
     <t>ILLIMITY BANK SPA</t>
   </si>
   <si>
-    <t>815600A029117B20DD63</t>
-  </si>
-  <si>
     <t>IT0005359192</t>
   </si>
   <si>
     <t>INDUSTRIE DE NORA SPA</t>
   </si>
   <si>
-    <t>815600CD933CB2F89862</t>
-  </si>
-  <si>
     <t>IT0005186371</t>
   </si>
   <si>
@@ -302,45 +251,30 @@
     <t>INFRASTRUTTURE WIRELESS ITALIANE SPA - INWIT</t>
   </si>
   <si>
-    <t>81560066183FE361C071</t>
-  </si>
-  <si>
     <t>IT0005090300</t>
   </si>
   <si>
     <t>Iveco Group N.V.</t>
   </si>
   <si>
-    <t>549300ZWF2ZJDD9EOR96</t>
-  </si>
-  <si>
     <t>NL0015000LU4</t>
   </si>
   <si>
     <t>JUVENTUS FOOTBALL CLUB SPA</t>
   </si>
   <si>
-    <t>815600A253A0AF58C166</t>
-  </si>
-  <si>
     <t>IT0005572778</t>
   </si>
   <si>
     <t>LEONARDO - SPA</t>
   </si>
   <si>
-    <t>529900X4EEX1U9LN3U39</t>
-  </si>
-  <si>
     <t>IT0003856405</t>
   </si>
   <si>
     <t>MARR SPA</t>
   </si>
   <si>
-    <t>815600576D5536AC7B34</t>
-  </si>
-  <si>
     <t>IT0003428445</t>
   </si>
   <si>
@@ -353,9 +287,6 @@
     <t>MFE-MEDIAFOREUROPE N.V.</t>
   </si>
   <si>
-    <t>213800DIFN7NR7B97A50</t>
-  </si>
-  <si>
     <t>NL0015001OJ9</t>
   </si>
   <si>
@@ -368,27 +299,18 @@
     <t>OVS SPA</t>
   </si>
   <si>
-    <t>8156001A772766DCAA71</t>
-  </si>
-  <si>
     <t>IT0005043507</t>
   </si>
   <si>
     <t>PIAGGIO &amp; C. SPA</t>
   </si>
   <si>
-    <t>8156000256C2431C2E92</t>
-  </si>
-  <si>
     <t>IT0003073266</t>
   </si>
   <si>
     <t>SAES GETTERS SPA</t>
   </si>
   <si>
-    <t>81560035783FD9E2E641</t>
-  </si>
-  <si>
     <t>IT0001029492</t>
   </si>
   <si>
@@ -401,9 +323,6 @@
     <t>SAIPEM SPA</t>
   </si>
   <si>
-    <t>549300PHV8MBDHWB8X12</t>
-  </si>
-  <si>
     <t>IT0005495657</t>
   </si>
   <si>
@@ -416,9 +335,6 @@
     <t>SALVATORE FERRAGAMO SPA</t>
   </si>
   <si>
-    <t>5493005GRP0FEE3NRI35</t>
-  </si>
-  <si>
     <t>IT0004712375</t>
   </si>
   <si>
@@ -431,45 +347,30 @@
     <t>SANLORENZO SPA</t>
   </si>
   <si>
-    <t>8156006C71E895860132</t>
-  </si>
-  <si>
     <t>IT0003549422</t>
   </si>
   <si>
     <t>SECO SPA</t>
   </si>
   <si>
-    <t>8156008C44408AB6D716</t>
-  </si>
-  <si>
     <t>IT0005438046</t>
   </si>
   <si>
     <t>SESA SPA</t>
   </si>
   <si>
-    <t>81560005C031D4E76707</t>
-  </si>
-  <si>
     <t>IT0004729759</t>
   </si>
   <si>
     <t>ST MICROELECTRONICS NV</t>
   </si>
   <si>
-    <t>213800Z8NOHIKRI42W10</t>
-  </si>
-  <si>
     <t>NL0000226223</t>
   </si>
   <si>
     <t>TECHNOPROBE</t>
   </si>
   <si>
-    <t>8156007154CD8334D053</t>
-  </si>
-  <si>
     <t>IT0005482333</t>
   </si>
   <si>
@@ -482,18 +383,12 @@
     <t>TELECOM ITALIA SPA</t>
   </si>
   <si>
-    <t>549300W384M3RI3VXU42</t>
-  </si>
-  <si>
     <t>IT0003497168</t>
   </si>
   <si>
     <t>UNIEURO SPA</t>
   </si>
   <si>
-    <t>815600583BE5BC67EB82</t>
-  </si>
-  <si>
     <t>IT0005239881</t>
   </si>
   <si>
@@ -506,9 +401,6 @@
     <t>WEBUILD SPA</t>
   </si>
   <si>
-    <t>549300UKR289DF4UXQ47</t>
-  </si>
-  <si>
     <t>IT0003865570</t>
   </si>
   <si>
@@ -525,14 +417,27 @@
   </si>
   <si>
     <t>17/05/2024</t>
+  </si>
+  <si>
+    <t>Formatted Number</t>
+  </si>
+  <si>
+    <t>Invalid Date</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>xxx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -563,9 +468,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -903,10 +809,18 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" customWidth="1"/>
+    <col min="7" max="7" width="33.1640625" customWidth="1"/>
+    <col min="8" max="8" width="16.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -919,1277 +833,1277 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>132</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1">
+        <v>1.2345676789</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
       <c r="F2">
         <v>0.5</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="2">
         <v>45148</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.999</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
       </c>
       <c r="F3">
         <v>0.69</v>
       </c>
-      <c r="G3" s="1">
-        <v>45421</v>
+      <c r="G3" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" s="1">
+        <v>1.2345676789</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
       </c>
       <c r="F4">
         <v>1.27</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
         <v>45384</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.2345676789</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
       </c>
       <c r="F5">
         <v>0.59</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2">
         <v>45425</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F6">
         <v>1.57</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>45177</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F7">
         <v>1.02</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
         <v>44061</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F8">
         <v>0.8</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
         <v>45419</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
+        <v>32</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F9">
         <v>0.54</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="2">
         <v>45427</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" t="s">
-        <v>44</v>
+        <v>36</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F10">
         <v>0.51</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
         <v>45309</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" t="s">
-        <v>44</v>
+        <v>36</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F11">
         <v>0.68</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
         <v>45422</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F12">
         <v>0.64</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2">
         <v>45385</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F13">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="2">
         <v>45426</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" t="s">
-        <v>51</v>
+        <v>42</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F14">
         <v>0.71</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="2">
         <v>45386</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" t="s">
-        <v>59</v>
+        <v>49</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F15">
         <v>0.6</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2">
         <v>45350</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" t="s">
-        <v>62</v>
+        <v>51</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F16">
         <v>0.95</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="2">
         <v>45359</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" t="s">
-        <v>62</v>
+        <v>51</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F17">
         <v>0.96</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="2">
         <v>45401</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" t="s">
-        <v>62</v>
+        <v>51</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F18">
         <v>0.59</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="2">
         <v>45420</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" t="s">
-        <v>69</v>
+        <v>57</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="F19">
         <v>0.59</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="2">
         <v>45420</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" t="s">
-        <v>74</v>
+        <v>61</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="F20">
         <v>0.59</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="2">
         <v>44881</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" t="s">
-        <v>74</v>
+        <v>61</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="F21">
         <v>1.7</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="2">
         <v>45358</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" t="s">
-        <v>77</v>
+        <v>63</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E22" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F22">
         <v>0.8</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="2">
         <v>45237</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" t="s">
-        <v>80</v>
+        <v>65</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E23" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="F23">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="2">
         <v>45420</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" t="s">
-        <v>83</v>
+        <v>67</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E24" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="F24">
         <v>0.5</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="2">
         <v>45418</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" t="s">
-        <v>83</v>
+        <v>67</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E25" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="F25">
         <v>0.62</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="2">
         <v>45419</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" t="s">
-        <v>86</v>
+        <v>69</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E26" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="F26">
         <v>0.5</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="2">
         <v>45379</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" t="s">
-        <v>86</v>
+        <v>69</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E27" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="F27">
         <v>0.73</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="2">
         <v>45419</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="C28" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" t="s">
-        <v>86</v>
+        <v>69</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E28" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="F28">
         <v>0.72</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="2">
         <v>45029</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" t="s">
-        <v>86</v>
+        <v>69</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E29" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="F29">
         <v>0.69</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="2">
         <v>45385</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" t="s">
-        <v>93</v>
+        <v>75</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E30" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="F30">
         <v>0.7</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="2">
         <v>45212</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" t="s">
-        <v>96</v>
+        <v>77</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E31" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="F31">
         <v>0.7</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="2">
         <v>45420</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
         <v>7</v>
       </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
       <c r="C32" t="s">
-        <v>98</v>
-      </c>
-      <c r="D32" t="s">
-        <v>99</v>
+        <v>79</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E32" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F32">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="2">
         <v>45387</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
-      </c>
-      <c r="D33" t="s">
-        <v>99</v>
+        <v>79</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E33" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F33">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="2">
         <v>45427</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
-      </c>
-      <c r="D34" t="s">
-        <v>102</v>
+        <v>81</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E34" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="F34">
         <v>1.18</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="2">
         <v>45427</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" t="s">
-        <v>105</v>
+        <v>83</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E35" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="F35">
         <v>0.5</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G35" s="2">
         <v>45392</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="C36" t="s">
-        <v>109</v>
-      </c>
-      <c r="D36" t="s">
-        <v>110</v>
+        <v>87</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E36" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="F36">
         <v>0.81</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G36" s="2">
         <v>45272</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="B37" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="C37" t="s">
-        <v>114</v>
-      </c>
-      <c r="D37" t="s">
-        <v>115</v>
+        <v>91</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E37" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="F37">
         <v>1.02</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G37" s="2">
         <v>45414</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>114</v>
-      </c>
-      <c r="D38" t="s">
-        <v>115</v>
+        <v>91</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E38" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="F38">
         <v>0.81</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G38" s="2">
         <v>45412</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>117</v>
-      </c>
-      <c r="D39" t="s">
-        <v>118</v>
+        <v>93</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E39" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="F39">
         <v>0.71</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39" s="2">
         <v>45397</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C40" t="s">
-        <v>120</v>
-      </c>
-      <c r="D40" t="s">
-        <v>121</v>
+        <v>95</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E40" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="F40">
         <v>0.7</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40" s="2">
         <v>45422</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="B41" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
-      </c>
-      <c r="D41" t="s">
-        <v>121</v>
+        <v>95</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E41" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="F41">
         <v>0.5</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G41" s="2">
         <v>45422</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>125</v>
-      </c>
-      <c r="D42" t="s">
-        <v>126</v>
+        <v>99</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E42" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="F42">
         <v>1.21</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G42" s="2">
         <v>45364</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
-      </c>
-      <c r="D43" t="s">
-        <v>126</v>
+        <v>99</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E43" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="F43">
         <v>1.33</v>
       </c>
-      <c r="G43" s="1">
+      <c r="G43" s="2">
         <v>45387</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C44" t="s">
-        <v>125</v>
-      </c>
-      <c r="D44" t="s">
-        <v>126</v>
+        <v>99</v>
+      </c>
+      <c r="D44" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E44" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="F44">
         <v>0.7</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G44" s="2">
         <v>45420</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>125</v>
-      </c>
-      <c r="D45" t="s">
-        <v>126</v>
+        <v>99</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E45" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="F45">
         <v>0.6</v>
       </c>
-      <c r="G45" s="1">
+      <c r="G45" s="2">
         <v>45418</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>130</v>
-      </c>
-      <c r="D46" t="s">
-        <v>131</v>
+        <v>103</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E46" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="F46">
         <v>0.53</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G46" s="2">
         <v>45426</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="B47" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="C47" t="s">
-        <v>135</v>
-      </c>
-      <c r="D47" t="s">
-        <v>136</v>
+        <v>107</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E47" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="F47">
         <v>0.68</v>
       </c>
-      <c r="G47" s="1">
+      <c r="G47" s="2">
         <v>45370</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
         <v>7</v>
       </c>
-      <c r="B48" t="s">
-        <v>8</v>
-      </c>
       <c r="C48" t="s">
-        <v>138</v>
-      </c>
-      <c r="D48" t="s">
-        <v>139</v>
+        <v>109</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E48" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="F48">
         <v>0.5</v>
       </c>
-      <c r="G48" s="1">
+      <c r="G48" s="2">
         <v>45372</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C49" t="s">
-        <v>141</v>
-      </c>
-      <c r="D49" t="s">
-        <v>142</v>
+        <v>111</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E49" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="F49">
         <v>0.66</v>
       </c>
-      <c r="G49" s="1">
+      <c r="G49" s="2">
         <v>45372</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C50" t="s">
-        <v>144</v>
-      </c>
-      <c r="D50" t="s">
-        <v>145</v>
+        <v>113</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E50" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="F50">
         <v>0.6</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G50" s="2">
         <v>45420</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>147</v>
-      </c>
-      <c r="D51" t="s">
-        <v>148</v>
+        <v>115</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E51" t="s">
-        <v>149</v>
+        <v>116</v>
       </c>
       <c r="F51">
         <v>0.59</v>
       </c>
-      <c r="G51" s="1">
+      <c r="G51" s="2">
         <v>45315</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="B52" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="C52" t="s">
-        <v>152</v>
-      </c>
-      <c r="D52" t="s">
-        <v>153</v>
+        <v>119</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E52" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="F52">
         <v>0.79</v>
       </c>
-      <c r="G52" s="1">
+      <c r="G52" s="2">
         <v>45405</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>152</v>
-      </c>
-      <c r="D53" t="s">
-        <v>153</v>
+        <v>119</v>
+      </c>
+      <c r="D53" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E53" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="F53">
         <v>0.59</v>
       </c>
-      <c r="G53" s="1">
+      <c r="G53" s="2">
         <v>45428</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C54" t="s">
-        <v>155</v>
-      </c>
-      <c r="D54" t="s">
-        <v>156</v>
+        <v>121</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E54" t="s">
-        <v>157</v>
+        <v>122</v>
       </c>
       <c r="F54">
         <v>0.59</v>
       </c>
-      <c r="G54" s="1">
+      <c r="G54" s="2">
         <v>45407</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
       <c r="B55" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="C55" t="s">
-        <v>160</v>
-      </c>
-      <c r="D55" t="s">
-        <v>161</v>
+        <v>125</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E55" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="F55">
         <v>0.77</v>
       </c>
-      <c r="G55" s="1">
+      <c r="G55" s="2">
         <v>44623</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>163</v>
+        <v>127</v>
       </c>
       <c r="B56" t="s">
-        <v>164</v>
+        <v>128</v>
       </c>
       <c r="C56" t="s">
-        <v>160</v>
-      </c>
-      <c r="D56" t="s">
-        <v>161</v>
+        <v>125</v>
+      </c>
+      <c r="D56" s="1">
+        <v>1.2345676789</v>
       </c>
       <c r="E56" t="s">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="F56">
         <v>0.5</v>
       </c>
-      <c r="G56" s="1">
+      <c r="G56" s="2">
         <v>45281</v>
       </c>
     </row>
@@ -2208,17 +2122,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>